<commit_message>
Experiment with bar charts
</commit_message>
<xml_diff>
--- a/data/ArticlesByCategory.xlsx
+++ b/data/ArticlesByCategory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PhD\Literature Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvall\PycharmProjects\learning-sequences-review\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29036083-E68D-4516-95BE-4FC415AF7561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D8369-ED4C-420A-8DF4-21D4AED475BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{D7484189-93F7-4265-9FF5-ABF511346522}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{D7484189-93F7-4265-9FF5-ABF511346522}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="153">
   <si>
     <t>Domain</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Akhuseyinoglu et al_2021_Data-drive',</t>
   </si>
   <si>
-    <t>Applied</t>
-  </si>
-  <si>
     <t>Programming</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
   </si>
   <si>
     <t>Owen et al_2016_Modeling',</t>
-  </si>
-  <si>
-    <t>Game</t>
   </si>
   <si>
     <t>Task Success</t>
@@ -599,6 +593,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -606,7 +607,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -621,6 +622,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -649,20 +657,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -976,555 +970,536 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9566F0-9569-43E9-BE2A-D05E7321400D}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H38" sqref="H38"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.68359375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.15625" customWidth="1"/>
-    <col min="5" max="5" width="12.5234375" customWidth="1"/>
-    <col min="6" max="6" width="11.47265625" customWidth="1"/>
-    <col min="7" max="7" width="12.15625" customWidth="1"/>
-    <col min="8" max="8" width="15.7890625" customWidth="1"/>
-    <col min="9" max="9" width="14.578125" customWidth="1"/>
-    <col min="10" max="10" width="10.578125" customWidth="1"/>
-    <col min="12" max="12" width="11.7890625" customWidth="1"/>
-    <col min="13" max="13" width="13.3125" customWidth="1"/>
-    <col min="14" max="14" width="10.734375" customWidth="1"/>
-    <col min="15" max="15" width="11.20703125" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" customWidth="1"/>
+    <col min="5" max="5" width="11.46484375" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.59765625" customWidth="1"/>
+    <col min="9" max="9" width="10.59765625" customWidth="1"/>
+    <col min="11" max="11" width="11.796875" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.73046875" customWidth="1"/>
+    <col min="14" max="14" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="D1" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>130</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="B12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="D13" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
@@ -1533,1293 +1508,1239 @@
         <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="L14" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="64.5" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="64.5" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D18" s="1" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="I18" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="64.5" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="64.5" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="D21" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="87" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="90" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D23" s="1" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D24" s="1" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D26" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="52.9" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D28" s="1" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D29" s="1" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="39" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D32" s="1" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D33" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="O33" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>134</v>
+      </c>
+      <c r="N33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>130</v>
+        <v>23</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="64.5" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D35" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D37" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>145</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="51.75" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>133</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D41" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>82</v>
+      <c r="C43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D44" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="39" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D45" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46" s="4"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2828,53 +2749,52 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H46">
     <sortCondition ref="A2:A46"/>
   </sortState>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Guided">
-      <formula>NOT(ISERROR(SEARCH("Guided",E1)))</formula>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Problem">
+      <formula>NOT(ISERROR(SEARCH("Problem",D1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Knowledge">
-      <formula>NOT(ISERROR(SEARCH("Knowledge",E1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Knowledge",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="Problem">
-      <formula>NOT(ISERROR(SEARCH("Problem",E1)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="Guided">
+      <formula>NOT(ISERROR(SEARCH("Guided",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Metaco">
-      <formula>NOT(ISERROR(SEARCH("Metaco",H1)))</formula>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Learn">
+      <formula>NOT(ISERROR(SEARCH("Learn",G1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Problem">
-      <formula>NOT(ISERROR(SEARCH("Problem",H1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Problem",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Learn">
-      <formula>NOT(ISERROR(SEARCH("Learn",H1)))</formula>
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Metaco">
+      <formula>NOT(ISERROR(SEARCH("Metaco",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Natural">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Formal">
+      <formula>NOT(ISERROR(SEARCH("Formal",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Natural">
       <formula>NOT(ISERROR(SEARCH("Natural",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Formal">
-      <formula>NOT(ISERROR(SEARCH("Formal",B1)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Deep">
+      <formula>NOT(ISERROR(SEARCH("Deep",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Knowl">
+      <formula>NOT(ISERROR(SEARCH("Knowl",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Knowl">
-      <formula>NOT(ISERROR(SEARCH("Knowl",J1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Deep">
-      <formula>NOT(ISERROR(SEARCH("Deep",J1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Meso">
-      <formula>NOT(ISERROR(SEARCH("Meso",K1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Meso",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added link test in table, Select complete row in table
</commit_message>
<xml_diff>
--- a/data/ArticlesByCategory.xlsx
+++ b/data/ArticlesByCategory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvall\Pycharm Projects\learning-sequences-review\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997B4F6A-32F6-4A38-81A0-DC46EE618CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D7142A-05D0-4FC9-B901-8B8019DE7BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{D7484189-93F7-4265-9FF5-ABF511346522}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>History</t>
   </si>
   <si>
-    <t>Akhuseyinoglu et al_2021_Data-drive',</t>
-  </si>
-  <si>
     <t>Programming</t>
   </si>
   <si>
@@ -495,6 +492,9 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>[Akhuseyinoglu, K., &amp; Brusilovsky, P. (2021). Data-driven modeling of learners’ individual differences for predicting engagement and success in online learning](https://www.doi.org/10.1145/3450613.3456834)</t>
   </si>
 </sst>
 </file>
@@ -974,7 +974,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K4" sqref="K4"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -995,7 +995,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1013,45 +1013,45 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="87" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -1060,19 +1060,19 @@
         <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
@@ -1086,10 +1086,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>15</v>
@@ -1098,144 +1098,144 @@
         <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -1244,10 +1244,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
@@ -1256,24 +1256,24 @@
         <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -1282,303 +1282,303 @@
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -1587,77 +1587,77 @@
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>10</v>
@@ -1666,110 +1666,110 @@
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K19" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="62.4" x14ac:dyDescent="0.55000000000000004">
@@ -1780,13 +1780,13 @@
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -1795,98 +1795,98 @@
         <v>12</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="87" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K22" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K23" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
@@ -1900,77 +1900,77 @@
         <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>10</v>
@@ -1979,86 +1979,86 @@
         <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>15</v>
@@ -2067,24 +2067,24 @@
         <v>12</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -2093,150 +2093,150 @@
         <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K30" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K31" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="K32" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>10</v>
@@ -2245,115 +2245,115 @@
         <v>14</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="K33" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>10</v>
@@ -2362,36 +2362,36 @@
         <v>14</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>10</v>
@@ -2400,159 +2400,159 @@
         <v>14</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K37" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="50.1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K38" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="K39" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K40" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M40" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>10</v>
@@ -2561,112 +2561,112 @@
         <v>14</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="K41" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J42" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K42" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>10</v>
@@ -2675,36 +2675,36 @@
         <v>14</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I44" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="K44" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="37.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>10</v>
@@ -2713,10 +2713,10 @@
         <v>14</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>11</v>
@@ -2725,19 +2725,19 @@
         <v>12</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">

</xml_diff>